<commit_message>
*********** Release 110-FFFF-00-00-01-00 *****************
*) Add low-level MDIO frame commands supporting for USBXpress;
*) Change password to RS style;
</commit_message>
<xml_diff>
--- a/doc/Design/USBXpress_Frame.xlsx
+++ b/doc/Design/USBXpress_Frame.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenSource\c8051f340_base\doc\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenSource\silabs_c2adapter\doc\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1956" yWindow="0" windowWidth="2160" windowHeight="0"/>
+    <workbookView xWindow="2976" yWindow="0" windowWidth="2160" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Frame Brief" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>(2B)</t>
   </si>
@@ -470,6 +470,43 @@
   </si>
   <si>
     <t>C2M Flash Page Erase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1120</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1121</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data
+(2B)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1122</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1123</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDIOM FramePRIA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDIOM FrameRead</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDIOM FrameWrite</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDIOM FrameAddr</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -647,10 +684,49 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,91 +736,61 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1029,96 +1075,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U71" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="27" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" style="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="27"/>
+    <col min="1" max="1" width="15.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="16" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="32" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1137,384 +1183,468 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T89" sqref="T89"/>
+      <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="27"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="35"/>
+      <c r="B11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="27"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18" t="s">
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18" t="s">
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21"/>
-    </row>
-    <row r="18" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18" t="s">
+      <c r="E22" s="25"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F23" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="25"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18" t="s">
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F24" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="23"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F19:H19"/>
+  <mergeCells count="23">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="A10:A17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>